<commit_message>
1) Revert "Update checklist.xlsx"  - 데이터를 덮어 쓴 잘못된 커밋을 제거
This reverts commit c2b9eef846243d2120ec7d92820b84aabc9c91a1.
</commit_message>
<xml_diff>
--- a/CheckList/checklist.xlsx
+++ b/CheckList/checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wousi\OneDrive\문서\GitHub\financial-statements\CheckList\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B711C5-AA43-48CA-91C8-05755C6B22CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6024B227-AC67-4F77-916A-31D0B54AB92B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2232" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{38E45DD5-6008-40C8-ABF5-363B69EF7224}"/>
+    <workbookView xWindow="1056" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{38E45DD5-6008-40C8-ABF5-363B69EF7224}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="143">
   <si>
     <t>재무상태표</t>
   </si>
@@ -472,14 +473,6 @@
   </si>
   <si>
     <t>부국증권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>상상인증권</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>판관비값있으나 raw데이타에없음</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -884,50 +877,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>75</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>87</xdr:col>
-      <xdr:colOff>115185</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>92339</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="8" name="그림 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E0BA10-90F5-40E1-80F6-AC47E17B9CC5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="54711600" y="441960"/>
-          <a:ext cx="8161905" cy="8047619"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1228,10 +1177,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27EB292-3771-4589-8377-3EAE80F370EF}">
-  <dimension ref="A1:BY125"/>
+  <dimension ref="A1:BL125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BW1" workbookViewId="0">
-      <selection activeCell="CK10" sqref="CK10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -1243,7 +1192,7 @@
     <col min="5" max="5" width="23.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>131</v>
       </c>
@@ -1260,7 +1209,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1303,14 +1252,8 @@
       <c r="BL2" t="s">
         <v>142</v>
       </c>
-      <c r="BX2">
-        <v>9</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:77" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1327,7 +1270,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1344,7 +1287,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="5" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
@@ -1361,7 +1304,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A6" s="5" t="s">
         <v>9</v>
       </c>
@@ -1378,7 +1321,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:77" ht="52.2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:64" ht="52.2" x14ac:dyDescent="0.4">
       <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
@@ -1395,7 +1338,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
@@ -1412,7 +1355,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="9" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -1425,11 +1368,8 @@
       <c r="D9" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="E9" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="10" spans="1:77" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A10" s="5" t="s">
         <v>13</v>
       </c>
@@ -1443,7 +1383,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
@@ -1457,7 +1397,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1471,7 +1411,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1485,7 +1425,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
         <v>17</v>
       </c>
@@ -1499,7 +1439,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="15" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
@@ -1513,7 +1453,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:77" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:64" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
@@ -3056,7 +2996,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>